<commit_message>
Add the HIV PPI reporting template
</commit_message>
<xml_diff>
--- a/HIV_PPI_map_template.xlsx
+++ b/HIV_PPI_map_template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amstutzal/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amstutzal/Documents/GitHub/quarto-website-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8E451EE-EA40-B74F-B9E8-FE6CB2566A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931FE96C-EE6E-C94D-8104-A149734A5F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="29400" windowHeight="17400" xr2:uid="{D12A7DC9-9E3F-7F4D-A9DC-A49EAD0313CF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Prospective Clinical Trial" sheetId="2" r:id="rId1"/>
+    <sheet name="PPI description" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -37,16 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Example for Strategy</t>
-  </si>
-  <si>
-    <t>Add References and Links</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Project title</t>
   </si>
@@ -109,13 +100,19 @@
   </si>
   <si>
     <t>All phases</t>
+  </si>
+  <si>
+    <t>Provide a clear description of how PPI was implemented in the study</t>
+  </si>
+  <si>
+    <t>Add references and links to the project and/or further explanation of how PPI was implemented in the study</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,13 +157,6 @@
     </font>
     <font>
       <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <name val="Candara"/>
       <family val="2"/>
     </font>
@@ -181,11 +171,6 @@
       <color rgb="FF7030A0"/>
       <name val="Candara"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF2A2A2A"/>
-      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -217,97 +202,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -633,62 +574,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A937B368-6BA3-114A-B184-8E5DAF134489}">
-  <dimension ref="A1:L125"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="58" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="58" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58" style="36" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="36" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="77.5" style="37" customWidth="1"/>
-    <col min="5" max="5" width="44.1640625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="54.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="256" style="17" customWidth="1"/>
-    <col min="8" max="8" width="51.6640625" style="38" customWidth="1"/>
-    <col min="9" max="9" width="90" style="38" customWidth="1"/>
-    <col min="10" max="10" width="50.1640625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="72.5" style="17" customWidth="1"/>
-    <col min="12" max="12" width="50.1640625" style="17" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="17"/>
+    <col min="1" max="1" width="41.6640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="34" style="19" customWidth="1"/>
+    <col min="4" max="4" width="77.5" style="20" customWidth="1"/>
+    <col min="5" max="5" width="44.1640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="54.33203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="96.5" style="13" customWidth="1"/>
+    <col min="8" max="8" width="84.1640625" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="9" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
@@ -696,10 +630,8 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" s="9" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="127" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -707,11 +639,9 @@
       <c r="E3" s="4"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" s="9" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" s="7" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -719,11 +649,9 @@
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -731,586 +659,309 @@
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-    </row>
-    <row r="12" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="13" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="11"/>
-    </row>
-    <row r="16" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="21"/>
-    </row>
-    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="21"/>
-    </row>
-    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="24"/>
-      <c r="K21" s="25"/>
-    </row>
-    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="24"/>
-    </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="26"/>
-    </row>
-    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="26"/>
-    </row>
-    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="27"/>
-    </row>
-    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-    </row>
-    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-    </row>
-    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-    </row>
-    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-    </row>
-    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-    </row>
-    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-    </row>
-    <row r="33" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-    </row>
-    <row r="34" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-    </row>
-    <row r="35" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-    </row>
-    <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-    </row>
-    <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-    </row>
-    <row r="38" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-    </row>
-    <row r="39" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-    </row>
-    <row r="40" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-    </row>
-    <row r="41" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-    </row>
-    <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-    </row>
-    <row r="43" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-    </row>
-    <row r="44" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-    </row>
-    <row r="45" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-    </row>
-    <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-    </row>
-    <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-    </row>
-    <row r="48" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-    </row>
-    <row r="49" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="28"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-    </row>
-    <row r="50" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="28"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="30"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-    </row>
-    <row r="51" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="28"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-    </row>
-    <row r="52" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="28"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-    </row>
-    <row r="53" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="32"/>
-      <c r="I53" s="32"/>
-    </row>
-    <row r="54" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="28"/>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-    </row>
-    <row r="55" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="28"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-    </row>
-    <row r="56" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="28"/>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-    </row>
-    <row r="57" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+    </row>
+    <row r="38" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+    </row>
+    <row r="48" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+    </row>
+    <row r="49" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+    </row>
+    <row r="50" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+    </row>
+    <row r="54" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+    </row>
+    <row r="55" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="63" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="4:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="65" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="66" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="67" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1412,60 +1063,60 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1679,6 +1330,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Confidentiality xmlns="8afd58ea-34e0-468c-a1a9-1a451fe987c3">Intern</Confidentiality>
@@ -1689,15 +1349,6 @@
     <TaxCatchAll xmlns="8afd58ea-34e0-468c-a1a9-1a451fe987c3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1720,6 +1371,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B2C2DC3-B697-4017-A9C6-64913115FAF3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87150991-2D7F-492E-8C7C-71183B323BBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1734,12 +1393,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B2C2DC3-B697-4017-A9C6-64913115FAF3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>